<commit_message>
added after each transaction status is updated to success or failed
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+  <si>
+    <t>CashIn</t>
+  </si>
   <si>
     <t>OnUsCheck</t>
   </si>
@@ -27,18 +30,23 @@
     <t>NotOnUsCheck</t>
   </si>
   <si>
-    <t>CashIn</t>
-  </si>
-  <si>
-    <t>Status</t>
+    <t>successful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +74,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,1197 +395,1213 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="1" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>911.07</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>231.36</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>10</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>897.56</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>528.85</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>180</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>382</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>997.34</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>32</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>484.04</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>388.6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>17</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>329.5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>669.55</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>374.31</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>445.64</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>86.43</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>682.58</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>599.98</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>872.16</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>446.53</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>778.83</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>662.42</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>184.2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>560.54999999999995</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>203.93</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>115.34</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>552.88</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>262.48</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>830.91</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>840.24</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>685.89</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>737.16</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>524.21</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>887.3</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>402.85</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>147.54</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>146</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>980.09</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>99.64</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>408.62</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>310.99</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>349.37</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>290.87</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>794.12</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>432.29</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>89.77</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>167.9</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>40.43</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>3.03</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>40.33</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>480.28</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>1105.1600000000001</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>248.6</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>966.68</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>192.68</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>697.58</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>165.16</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>304.37</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>426.8</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>106.36</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>506.71</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>878.65</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>74.260000000000005</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>612.35</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>974.04</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>262.64999999999998</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>305.12</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>280.29000000000002</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>83.1</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>434.59</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>49.06</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>398.31</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>526.61</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>1028.43</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>55.02</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>1162.4000000000001</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>926.47</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>395.63</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>794.99</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>147.79</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>546.57000000000005</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>151.47999999999999</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>95.84</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>618.70000000000005</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>136.19</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>406.6</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>640.78</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>906.25</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>83.67</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>981.34</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>194.22</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>31.34</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>782.26</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>646.75</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>476.8</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>815.39</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>418.73</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>279.61</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>449.09</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>1010.27</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>695.52</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>821.17</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>258</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>469.67</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>370.88</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
         <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>315.02</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>435.12</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>216.48</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>122.12</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>768.7</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>414.76</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
         <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>596.46</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>315.99</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
         <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>651.9</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>433.26</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
         <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>1174.8399999999999</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>97.28</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
         <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>796.79</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>701.84</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
         <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>268.70999999999998</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>416.74</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>617.01</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>703.2</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
         <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>822.66</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>871.06</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="1">
         <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>820.44</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>942.05</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="1">
         <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>272.49</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>376.82</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>602.49</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>528.11</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>474.16</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>183.81</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>546.38</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>784.96</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>566.1</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>602.41</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>1040.76</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>487.01</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
         <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>954.01</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>188.81</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="1">
         <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>984.71</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>460.21</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="1">
         <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>1031.6199999999999</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>567.16999999999996</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="1">
         <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>1066.32</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>12.99</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="1">
         <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="A74" s="1">
         <v>182.47</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>680.3</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="1">
         <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>22.68</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>829.99</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="1">
         <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>303.43</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>118.83</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="1">
         <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="1">
         <v>1018.31</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>819.3</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="1">
         <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>537.88</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>415.34</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="1">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79">
+      <c r="A79" s="1">
         <v>146.52000000000001</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>664.63</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80">
+      <c r="A80" s="1">
         <v>291.89999999999998</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>211.05</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="1">
         <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>142.65</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>495.96</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="1">
         <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
+      <c r="A82" s="1">
         <v>463.77</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>248.37</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="1">
         <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="A83" s="1">
         <v>427.98</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>863.94</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" s="1">
         <v>824.42</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>743.39</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="1">
         <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
+      <c r="A85" s="1">
         <v>389.71</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>267.2</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="1">
         <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>774.46</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>184.38</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="1">
         <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>1065.97</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>612.36</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
+      <c r="A88" s="1">
         <v>447.7</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>889.74</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="1">
         <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="A89" s="1">
         <v>245.68</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>601.69000000000005</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="1">
         <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="A90" s="1">
         <v>710.31</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>712.82</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
+      <c r="A91" s="1">
         <v>396.85</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>81.66</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
+      <c r="A92" s="1">
         <v>78.319999999999993</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>157.80000000000001</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="1">
         <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="A93" s="1">
         <v>173.05</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>359.43</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="1">
         <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94">
+      <c r="A94" s="1">
         <v>228.34</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>74.430000000000007</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="1">
         <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
+      <c r="A95" s="1">
         <v>240.81</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>399.58</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="1">
         <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>587.54999999999995</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>740.59</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="1">
         <v>170</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="A97" s="1">
         <v>312.13</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>23.37</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="1">
         <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98">
+      <c r="A98" s="1">
         <v>207.22</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>22.69</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="1">
         <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99">
+      <c r="A99" s="1">
         <v>237.25</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>213.42</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="1">
         <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>453.03</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>455.1</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="1">
         <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101">
+      <c r="A101" s="1">
         <v>266.18</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>593.36</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="1">
         <v>154</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102">
+      <c r="A102" s="1">
         <v>83.57</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>633.01</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="A103" s="1">
         <v>868.26</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
         <v>256.04000000000002</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="1">
         <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104">
+      <c r="A104" s="1">
         <v>452.2</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="1">
         <v>343.2</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="1">
         <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="A105" s="1">
         <v>793.94</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
         <v>400.73</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="1">
         <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106">
+      <c r="A106" s="1">
         <v>458.54</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>480.61</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="1">
         <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107">
+      <c r="A107" s="1">
         <v>430.26</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>383.35</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="1">
         <v>161</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>